<commit_message>
updates to readme and raw data
</commit_message>
<xml_diff>
--- a/GrandMeanData.xlsx
+++ b/GrandMeanData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="980" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="5440" yWindow="980" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="HumanInitiatorRTs" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="29">
   <si>
     <t>participant</t>
   </si>
@@ -112,7 +112,10 @@
     <t>DZT</t>
   </si>
   <si>
-    <t>Age</t>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Date of Experiment</t>
   </si>
 </sst>
 </file>
@@ -1614,13 +1617,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1631,964 +1634,1063 @@
         <v>27</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>101</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="C2">
-        <v>24</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="6">
+        <v>34074</v>
+      </c>
+      <c r="D2" s="6">
+        <v>42944</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>23</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>19</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>18</v>
       </c>
-      <c r="H2">
-        <v>15</v>
-      </c>
       <c r="I2">
+        <v>15</v>
+      </c>
+      <c r="J2">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>102</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C3">
-        <v>22</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="6">
+        <v>34660</v>
+      </c>
+      <c r="D3" s="6">
+        <v>42948</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E3">
-        <v>15</v>
-      </c>
       <c r="F3">
         <v>15</v>
       </c>
       <c r="G3">
+        <v>15</v>
+      </c>
+      <c r="H3">
         <v>17</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>11</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>12</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>103</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="C4">
-        <v>28</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="6">
+        <v>32404</v>
+      </c>
+      <c r="D4" s="6">
+        <v>42948</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>19</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>13</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>17</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>14</v>
       </c>
-      <c r="I4">
-        <v>15</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="J4">
+        <v>15</v>
+      </c>
+      <c r="L4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>104</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="C5">
-        <v>32</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="C5" s="6">
+        <v>31070</v>
+      </c>
+      <c r="D5" s="6">
+        <v>42949</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="5">
+      <c r="F5" s="5">
         <v>28</v>
       </c>
-      <c r="F5">
-        <v>15</v>
-      </c>
       <c r="G5">
+        <v>15</v>
+      </c>
+      <c r="H5">
         <v>17</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>14</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>17</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>105</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
+        <v>34336</v>
+      </c>
+      <c r="D6" s="6">
+        <v>42950</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="F6">
         <v>23</v>
       </c>
-      <c r="E6">
-        <v>23</v>
-      </c>
-      <c r="F6">
+      <c r="G6">
         <v>11</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>19</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>12</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>20</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>106</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7">
-        <v>26</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="C7" s="6">
+        <v>33405</v>
+      </c>
+      <c r="D7" s="6">
+        <v>42950</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>13</v>
       </c>
-      <c r="F7">
-        <v>15</v>
-      </c>
       <c r="G7">
+        <v>15</v>
+      </c>
+      <c r="H7">
         <v>21</v>
       </c>
-      <c r="H7">
-        <v>15</v>
-      </c>
       <c r="I7">
+        <v>15</v>
+      </c>
+      <c r="J7">
         <v>20</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>107</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="C8">
-        <v>33</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="C8" s="6">
+        <v>30727</v>
+      </c>
+      <c r="D8" s="6">
+        <v>42950</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>18</v>
       </c>
-      <c r="F8">
-        <v>15</v>
-      </c>
       <c r="G8">
+        <v>15</v>
+      </c>
+      <c r="H8">
         <v>16</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>13</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>108</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="C9">
-        <v>23</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="6">
+        <v>34435</v>
+      </c>
+      <c r="D9" s="6">
+        <v>42951</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>22</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>21</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>16</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>12</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>109</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
+        <v>33761</v>
+      </c>
+      <c r="D10" s="6">
+        <v>42951</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>14</v>
+      </c>
+      <c r="H10">
         <v>25</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10">
-        <v>10</v>
-      </c>
-      <c r="F10">
-        <v>14</v>
-      </c>
-      <c r="G10">
+      <c r="I10">
+        <v>13</v>
+      </c>
+      <c r="J10">
         <v>25</v>
       </c>
-      <c r="H10">
-        <v>13</v>
-      </c>
-      <c r="I10">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>110</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C11">
-        <v>26</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="C11" s="6">
+        <v>33382</v>
+      </c>
+      <c r="D11" s="6">
+        <v>42951</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>11</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>17</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>20</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>13</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>111</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C12">
-        <v>23</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="C12" s="6">
+        <v>34307</v>
+      </c>
+      <c r="D12" s="6">
+        <v>42951</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>18</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>16</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>18</v>
-      </c>
-      <c r="H12">
-        <v>16</v>
       </c>
       <c r="I12">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>112</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="C13">
-        <v>25</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="C13" s="6">
+        <v>33535</v>
+      </c>
+      <c r="D13" s="6">
+        <v>42954</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>23</v>
-      </c>
-      <c r="F13">
-        <v>18</v>
       </c>
       <c r="G13">
         <v>18</v>
       </c>
       <c r="H13">
+        <v>18</v>
+      </c>
+      <c r="I13">
         <v>9</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>113</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="C14">
-        <v>24</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="C14" s="6">
+        <v>33990</v>
+      </c>
+      <c r="D14" s="6">
+        <v>42954</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>16</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>13</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>20</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>13</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>114</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
-      <c r="C15">
-        <v>28</v>
-      </c>
-      <c r="D15" s="6" t="s">
+      <c r="C15" s="6">
+        <v>32476</v>
+      </c>
+      <c r="D15" s="6">
+        <v>42955</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>21</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>19</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>21</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>16</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>115</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="6">
+        <v>35338</v>
+      </c>
+      <c r="D16" s="6">
+        <v>42955</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16">
+      <c r="F16">
         <v>22</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>21</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>22</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>10</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>116</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="C17">
-        <v>20</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="C17" s="6">
+        <v>35301</v>
+      </c>
+      <c r="D17" s="6">
+        <v>42955</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>29</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>17</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>19</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>16</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>117</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
       </c>
-      <c r="C18">
-        <v>26</v>
-      </c>
-      <c r="D18" s="6" t="s">
+      <c r="C18" s="6">
+        <v>33099</v>
+      </c>
+      <c r="D18" s="6">
+        <v>42956</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="E18">
-        <v>14</v>
       </c>
       <c r="F18">
         <v>14</v>
       </c>
       <c r="G18">
+        <v>14</v>
+      </c>
+      <c r="H18">
         <v>17</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>14</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>118</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="6">
+        <v>34154</v>
+      </c>
+      <c r="D19" s="6">
+        <v>42956</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19">
+      <c r="F19">
         <v>22</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>14</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>17</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>11</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>119</v>
       </c>
       <c r="B20" t="s">
         <v>15</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="6">
+        <v>33782</v>
+      </c>
+      <c r="D20" s="6">
+        <v>42956</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20">
+      <c r="F20">
         <v>14</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>11</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>19</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>9</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>120</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
       </c>
-      <c r="C21">
-        <v>37</v>
-      </c>
-      <c r="D21" s="6" t="s">
+      <c r="C21" s="6">
+        <v>33956</v>
+      </c>
+      <c r="D21" s="6">
+        <v>42956</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E21">
-        <v>15</v>
-      </c>
       <c r="F21">
+        <v>15</v>
+      </c>
+      <c r="G21">
         <v>18</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>8</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>18</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>121</v>
       </c>
       <c r="B22" t="s">
         <v>16</v>
       </c>
-      <c r="C22">
-        <v>24</v>
-      </c>
-      <c r="D22" s="6" t="s">
+      <c r="C22" s="6">
+        <v>29148</v>
+      </c>
+      <c r="D22" s="6">
+        <v>42956</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>16</v>
       </c>
-      <c r="F22">
-        <v>15</v>
-      </c>
       <c r="G22">
+        <v>15</v>
+      </c>
+      <c r="H22">
         <v>20</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>12</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>122</v>
       </c>
       <c r="B23" t="s">
         <v>15</v>
       </c>
-      <c r="C23">
-        <v>27</v>
-      </c>
-      <c r="D23" s="6" t="s">
+      <c r="C23" s="6">
+        <v>32739</v>
+      </c>
+      <c r="D23" s="6">
+        <v>42957</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="E23">
-        <v>19</v>
       </c>
       <c r="F23">
         <v>19</v>
       </c>
       <c r="G23">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H23">
+        <v>15</v>
+      </c>
+      <c r="I23">
         <v>16</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>123</v>
       </c>
       <c r="B24" t="s">
         <v>15</v>
       </c>
-      <c r="C24">
-        <v>26</v>
-      </c>
-      <c r="D24" s="6" t="s">
+      <c r="C24" s="6">
+        <v>33251</v>
+      </c>
+      <c r="D24" s="6">
+        <v>42958</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>9</v>
-      </c>
-      <c r="F24">
-        <v>13</v>
       </c>
       <c r="G24">
         <v>13</v>
       </c>
       <c r="H24">
+        <v>13</v>
+      </c>
+      <c r="I24">
         <v>17</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>124</v>
       </c>
       <c r="B25" t="s">
         <v>15</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="6">
+        <v>33244</v>
+      </c>
+      <c r="D25" s="6">
+        <v>42958</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25">
-        <v>15</v>
-      </c>
       <c r="F25">
+        <v>15</v>
+      </c>
+      <c r="G25">
         <v>16</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>13</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>18</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>125</v>
       </c>
       <c r="B26" t="s">
         <v>15</v>
       </c>
-      <c r="C26">
-        <v>28</v>
-      </c>
-      <c r="D26" s="6" t="s">
+      <c r="C26" s="6">
+        <v>32700</v>
+      </c>
+      <c r="D26" s="6">
+        <v>42968</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>6</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>18</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>20</v>
       </c>
-      <c r="H26">
-        <v>15</v>
-      </c>
       <c r="I26">
+        <v>15</v>
+      </c>
+      <c r="J26">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>126</v>
       </c>
       <c r="B27" t="s">
         <v>15</v>
       </c>
-      <c r="C27">
-        <v>30</v>
-      </c>
-      <c r="D27" s="6" t="s">
+      <c r="C27" s="6">
+        <v>31989</v>
+      </c>
+      <c r="D27" s="6">
+        <v>42968</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>23</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>20</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>18</v>
-      </c>
-      <c r="H27">
-        <v>22</v>
       </c>
       <c r="I27">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>127</v>
       </c>
       <c r="B28" t="s">
         <v>16</v>
       </c>
-      <c r="C28">
-        <v>30</v>
-      </c>
-      <c r="D28" s="6" t="s">
+      <c r="C28" s="6">
+        <v>31655</v>
+      </c>
+      <c r="D28" s="6">
+        <v>42969</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>26</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>13</v>
       </c>
-      <c r="G28">
-        <v>15</v>
-      </c>
       <c r="H28">
+        <v>15</v>
+      </c>
+      <c r="I28">
         <v>12</v>
       </c>
-      <c r="I28">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>128</v>
       </c>
       <c r="B29" t="s">
         <v>15</v>
       </c>
-      <c r="C29">
-        <v>27</v>
-      </c>
-      <c r="D29" s="6" t="s">
+      <c r="C29" s="6">
+        <v>32837</v>
+      </c>
+      <c r="D29" s="6">
+        <v>42975</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>16</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>11</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>23</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>16</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>129</v>
       </c>
       <c r="B30" t="s">
         <v>16</v>
       </c>
-      <c r="C30">
-        <v>26</v>
-      </c>
-      <c r="D30" s="6" t="s">
+      <c r="C30" s="6">
+        <v>31726</v>
+      </c>
+      <c r="D30" s="6">
+        <v>42976</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>19</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>11</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>18</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>11</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>130</v>
       </c>
       <c r="B31" t="s">
         <v>16</v>
       </c>
-      <c r="C31">
-        <v>30</v>
-      </c>
-      <c r="D31" s="6" t="s">
+      <c r="C31" s="6">
+        <v>33313</v>
+      </c>
+      <c r="D31" s="6">
+        <v>42976</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>7</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>18</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>19</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>16</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>131</v>
       </c>
       <c r="B32" t="s">
         <v>15</v>
       </c>
-      <c r="C32">
-        <v>26</v>
-      </c>
-      <c r="D32" s="6" t="s">
+      <c r="C32" s="6">
+        <v>33478</v>
+      </c>
+      <c r="D32" s="6">
+        <v>42977</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>16</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>11</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>24</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>8</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>132</v>
       </c>
       <c r="B33" t="s">
         <v>15</v>
       </c>
-      <c r="C33">
-        <v>25</v>
-      </c>
-      <c r="D33" s="6" t="s">
+      <c r="C33" s="6">
+        <v>33844</v>
+      </c>
+      <c r="D33" s="6">
+        <v>42977</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>11</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>18</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>20</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>16</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>19</v>
       </c>
     </row>

</xml_diff>